<commit_message>
Update results and graphs
- update results with new shocks
- update graph code with plots that include "crop model"
- fix findEPQ to search instead by country instead of countryid
</commit_message>
<xml_diff>
--- a/crop_data/xlsx_data/B_C_US_shocks_c_s.xlsx
+++ b/crop_data/xlsx_data/B_C_US_shocks_c_s.xlsx
@@ -8,72 +8,33 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saket\GitHub\Climate-Ag-Simulation\crop_data\xlsx_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{639F67C1-81DA-497E-80C7-D53DC691035E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C9298FE-2ED4-4F34-8C64-C25F551F7C16}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25170" yWindow="2805" windowWidth="18030" windowHeight="11730" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20880" yWindow="2745" windowWidth="18030" windowHeight="11730" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Corn" sheetId="2" r:id="rId1"/>
     <sheet name="Soybean" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="24">
   <si>
     <t>region</t>
-  </si>
-  <si>
-    <t>r_yr1</t>
-  </si>
-  <si>
-    <t>r_yr2</t>
-  </si>
-  <si>
-    <t>r_yr3</t>
-  </si>
-  <si>
-    <t>r_yr4</t>
-  </si>
-  <si>
-    <t>r_yr5</t>
-  </si>
-  <si>
-    <t>r_yr6</t>
-  </si>
-  <si>
-    <t>r_yr7</t>
-  </si>
-  <si>
-    <t>r_yr8</t>
-  </si>
-  <si>
-    <t>r_yr9</t>
-  </si>
-  <si>
-    <t>r_yr10</t>
-  </si>
-  <si>
-    <t>r_yr11</t>
-  </si>
-  <si>
-    <t>r_yr12</t>
-  </si>
-  <si>
-    <t>r_yr13</t>
-  </si>
-  <si>
-    <t>r_yr14</t>
-  </si>
-  <si>
-    <t>r_yr15</t>
   </si>
   <si>
     <t>China</t>
@@ -466,8 +427,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E21FB581-8CBB-449F-BF10-524CEB790D58}">
   <dimension ref="A1:Q24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -479,55 +440,69 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1">
+        <f>C1+1</f>
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1">
+        <f t="shared" ref="E1:Q1" si="0">D1+1</f>
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1">
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1">
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1">
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1">
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1">
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1">
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1">
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1">
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1">
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1">
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1">
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="C2" s="1">
         <v>-6.4000000000000001E-2</v>
@@ -577,7 +552,7 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="C3" s="1">
         <v>-0.219</v>
@@ -627,7 +602,7 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="C4" s="1">
         <v>-0.04</v>
@@ -677,7 +652,7 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="C5" s="1">
         <v>-0.04</v>
@@ -727,7 +702,7 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="C6" s="1">
         <v>-0.04</v>
@@ -777,7 +752,7 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="C7" s="1">
         <v>-0.04</v>
@@ -827,7 +802,7 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="C8" s="1">
         <v>-0.04</v>
@@ -877,7 +852,7 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="C9" s="1">
         <v>-0.04</v>
@@ -927,7 +902,7 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="C10" s="1">
         <v>-0.04</v>
@@ -977,7 +952,7 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="C11" s="1">
         <v>-0.04</v>
@@ -1027,7 +1002,7 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="C12" s="1">
         <v>-0.04</v>
@@ -1077,7 +1052,7 @@
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="C13" s="1">
         <v>-0.04</v>
@@ -1127,7 +1102,7 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="C14" s="1">
         <v>-0.04</v>
@@ -1177,7 +1152,7 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="C15" s="1">
         <v>-0.04</v>
@@ -1227,7 +1202,7 @@
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="C16" s="1">
         <v>-0.04</v>
@@ -1277,7 +1252,7 @@
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="C17" s="1">
         <v>-0.04</v>
@@ -1327,7 +1302,7 @@
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="C18" s="1">
         <v>-0.04</v>
@@ -1377,7 +1352,7 @@
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="C19" s="1">
         <v>-0.04</v>
@@ -1427,7 +1402,7 @@
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="C20" s="1">
         <v>-0.04</v>
@@ -1477,7 +1452,7 @@
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="C21" s="1">
         <v>-0.04</v>
@@ -1527,7 +1502,7 @@
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="C22" s="1">
         <v>-0.04</v>
@@ -1577,7 +1552,7 @@
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="C23" s="1">
         <v>-0.04</v>
@@ -1627,7 +1602,7 @@
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="C24" s="1">
         <v>-0.04</v>
@@ -1684,8 +1659,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32A6C050-2288-4F3F-9151-5725A4EE8CCA}">
   <dimension ref="A1:Q24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1697,55 +1672,69 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1">
+        <f>C1+1</f>
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1">
+        <f t="shared" ref="E1:Q1" si="0">D1+1</f>
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1">
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1">
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1">
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1">
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1">
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1">
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1">
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1">
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1">
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1">
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1">
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="C2" s="1">
         <v>-0.185</v>
@@ -1795,7 +1784,7 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="C3" s="1">
         <v>-0.28899999999999998</v>
@@ -1845,7 +1834,7 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="C4" s="1">
         <v>-5.5E-2</v>
@@ -1895,7 +1884,7 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="C5" s="1">
         <v>-5.5E-2</v>
@@ -1945,7 +1934,7 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="C6" s="1">
         <v>-5.5E-2</v>
@@ -1995,7 +1984,7 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="C7" s="1">
         <v>-5.5E-2</v>
@@ -2045,7 +2034,7 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="C8" s="1">
         <v>-5.5E-2</v>
@@ -2095,7 +2084,7 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="C9" s="1">
         <v>-5.5E-2</v>
@@ -2145,7 +2134,7 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="C10" s="1">
         <v>-5.5E-2</v>
@@ -2195,7 +2184,7 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="C11" s="1">
         <v>-5.5E-2</v>
@@ -2245,7 +2234,7 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="C12" s="1">
         <v>-5.5E-2</v>
@@ -2295,7 +2284,7 @@
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="C13" s="1">
         <v>-5.5E-2</v>
@@ -2345,7 +2334,7 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="C14" s="1">
         <v>-5.5E-2</v>
@@ -2395,7 +2384,7 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="C15" s="1">
         <v>-5.5E-2</v>
@@ -2445,7 +2434,7 @@
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="C16" s="1">
         <v>-5.5E-2</v>
@@ -2495,7 +2484,7 @@
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="C17" s="1">
         <v>-5.5E-2</v>
@@ -2545,7 +2534,7 @@
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="C18" s="1">
         <v>-5.5E-2</v>
@@ -2595,7 +2584,7 @@
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="C19" s="1">
         <v>-5.5E-2</v>
@@ -2645,7 +2634,7 @@
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="C20" s="1">
         <v>-5.5E-2</v>
@@ -2695,7 +2684,7 @@
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="C21" s="1">
         <v>-5.5E-2</v>
@@ -2745,7 +2734,7 @@
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="C22" s="1">
         <v>-5.5E-2</v>
@@ -2795,7 +2784,7 @@
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="C23" s="1">
         <v>-5.5E-2</v>
@@ -2845,7 +2834,7 @@
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="C24" s="1">
         <v>-5.5E-2</v>

</xml_diff>